<commit_message>
Adjustments to velocity data and data fit + analysis.  There is currently an issue with the motor parameter values that the fit yields, since they are not realistic values.
</commit_message>
<xml_diff>
--- a/3 Wheel Robot Encoder Rotational Velocity Test Data.xlsx
+++ b/3 Wheel Robot Encoder Rotational Velocity Test Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RobotPhysics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF36EA4-2EFF-4AB4-9936-22C2D6546D22}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955DB4DA-7954-4F54-975F-32921A9B23A8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{83B8D388-A5D4-4412-9613-4A869FE96360}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{83B8D388-A5D4-4412-9613-4A869FE96360}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -22,6 +23,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,9 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B635A12E-6549-4C86-A74B-DC86FD5AB400}">
   <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2358,4 +2361,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FFBBD5-3139-45DA-9F36-22B7D31F8415}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>